<commit_message>
ECTEST TC24 and TC33 Update
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC24_Verify_PDP_Page.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC24_Verify_PDP_Page.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Vaibhav Oza\KAMAN_ECTEST_IE_SANITY-master\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="48">
   <si>
     <t>TestCase</t>
   </si>
@@ -114,9 +119,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>VERIFY_TEXT_PRESENT</t>
   </si>
   <si>
     <t>Price</t>
@@ -247,7 +249,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
@@ -268,6 +270,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -278,6 +281,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -326,7 +332,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -361,7 +367,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -572,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,7 +610,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>5</v>
@@ -616,21 +622,17 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>8</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="12" t="s">
+      <c r="A4" s="17"/>
+      <c r="B4" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="11"/>
@@ -642,8 +644,8 @@
       <c r="B5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>43</v>
+      <c r="C5" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>8</v>
@@ -652,11 +654,11 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="11"/>
-      <c r="D6" s="12"/>
+      <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -665,7 +667,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>8</v>
@@ -675,91 +677,77 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="11"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="C10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="11"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>18</v>
-      </c>
+      <c r="A11" s="5"/>
+      <c r="B11" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="11"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
-      <c r="B12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="6"/>
+      <c r="B12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
-      <c r="B13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="B13" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="6"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="11"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
@@ -767,88 +755,76 @@
         <v>16</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
-      <c r="B16" s="11" t="s">
-        <v>33</v>
+      <c r="B16" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>22</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
-      <c r="B18" s="11" t="s">
-        <v>33</v>
+      <c r="B18" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>23</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
-      <c r="B20" s="11" t="s">
-        <v>33</v>
+      <c r="B20" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -857,13 +833,13 @@
         <v>16</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -872,13 +848,13 @@
         <v>16</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -887,13 +863,13 @@
         <v>16</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -902,13 +878,13 @@
         <v>16</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -917,28 +893,28 @@
         <v>16</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="9" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -947,28 +923,28 @@
         <v>16</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="9" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1059,7 +1035,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,10 +1094,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1134,10 +1110,10 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1150,10 +1126,10 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="15" t="s">
         <v>37</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1166,7 +1142,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="19" t="b">
         <v>1</v>
@@ -1182,7 +1158,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="16" t="b">
         <v>1</v>
@@ -1198,7 +1174,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="18">
         <v>430049</v>
@@ -1214,10 +1190,10 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>